<commit_message>
Corrected silkscreen and minor change to top layer.
</commit_message>
<xml_diff>
--- a/PCB modules/breakout/harp expander breakout BOM.xlsx
+++ b/PCB modules/breakout/harp expander breakout BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB modules\breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4368AD-3AD2-48B4-B79B-7991B5174FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870A2D1-096F-409D-A8E2-133D1102B5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>1.5uF</t>
   </si>
   <si>
-    <t>SW1, SW2</t>
-  </si>
-  <si>
     <t>SWITCH</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>1658621-1</t>
+  </si>
+  <si>
+    <t>SW0, SW1</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1123,7 +1123,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -1174,11 +1174,11 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5">
         <v>1301.9306999999999</v>
@@ -1192,13 +1192,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
@@ -1209,13 +1209,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -1226,13 +1226,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
@@ -1243,13 +1243,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>14</v>
@@ -1284,10 +1284,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1295,10 +1295,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,12 +1306,12 @@
         <v>2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,20 +1319,20 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected wrong buttons polarity.
</commit_message>
<xml_diff>
--- a/PCB modules/breakout/harp expander breakout BOM.xlsx
+++ b/PCB modules/breakout/harp expander breakout BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB modules\breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229924C5-A90B-4F4D-9452-EBEEC7B33BED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEFC800-C90D-4DD9-B5FB-9BEFD55E7FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>C0603</t>
   </si>
   <si>
@@ -84,18 +81,6 @@
     <t>R3, R4</t>
   </si>
   <si>
-    <t>CR0603-JW-272ELF</t>
-  </si>
-  <si>
-    <t>2.7k</t>
-  </si>
-  <si>
-    <t>C1608X7S1C155K080AC</t>
-  </si>
-  <si>
-    <t>1.5uF</t>
-  </si>
-  <si>
     <t>SWITCH</t>
   </si>
   <si>
@@ -138,12 +123,6 @@
     <t>TERMINAL BLOBK PLUG 2WAY</t>
   </si>
   <si>
-    <t>CRGH0603J270R</t>
-  </si>
-  <si>
-    <t>270R 200mW</t>
-  </si>
-  <si>
     <t>IDC 10WAY STRAIGHT</t>
   </si>
   <si>
@@ -181,13 +160,34 @@
   </si>
   <si>
     <t>To create a cable with 0.5 meters</t>
+  </si>
+  <si>
+    <t>ERJ3GEYJ432V</t>
+  </si>
+  <si>
+    <t>ERJ3GEYJ222V</t>
+  </si>
+  <si>
+    <t>4.3k 100mW</t>
+  </si>
+  <si>
+    <t>2.2k 100mW</t>
+  </si>
+  <si>
+    <t>CL10A105KA8NNNC</t>
+  </si>
+  <si>
+    <t>1uF 25V</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +357,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -718,7 +724,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,6 +744,7 @@
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1105,7 +1112,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B3" sqref="B3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,12 +1142,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1153,59 +1160,61 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,17 +1222,17 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5">
         <v>1301.9306999999999</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,16 +1240,16 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1248,16 +1257,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,16 +1274,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1282,21 +1291,21 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1309,10 +1318,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,10 +1329,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1331,12 +1340,12 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1344,28 +1353,28 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1375,7 +1384,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1">
         <v>8</v>
@@ -1383,7 +1392,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1">
         <v>6</v>
@@ -1391,7 +1400,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1">
         <v>7</v>

</xml_diff>

<commit_message>
Updated files for final revision before production.
</commit_message>
<xml_diff>
--- a/PCB modules/breakout/harp expander breakout BOM.xlsx
+++ b/PCB modules/breakout/harp expander breakout BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB modules\breakout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEFC800-C90D-4DD9-B5FB-9BEFD55E7FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8947FE16-D899-426A-ACED-BA5461E146BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="4785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Qty</t>
   </si>
@@ -96,15 +96,6 @@
     <t>SBH11-PBPC-D05-ST-BK</t>
   </si>
   <si>
-    <t>20.155MH/8-E</t>
-  </si>
-  <si>
-    <t>20.1550M/8-E</t>
-  </si>
-  <si>
-    <t>20.1550M/2-E</t>
-  </si>
-  <si>
     <t>SV2</t>
   </si>
   <si>
@@ -117,12 +108,6 @@
     <t>TERMINAL BLOCK 2WAY</t>
   </si>
   <si>
-    <t>TERMINAL BLOBK PLUG 8WAY</t>
-  </si>
-  <si>
-    <t>TERMINAL BLOBK PLUG 2WAY</t>
-  </si>
-  <si>
     <t>IDC 10WAY STRAIGHT</t>
   </si>
   <si>
@@ -132,18 +117,12 @@
     <t>10 COND. 28AWG ROUND 1PC=100FT</t>
   </si>
   <si>
-    <t>517-3365/10</t>
-  </si>
-  <si>
     <t>SNT-100-BK-T</t>
   </si>
   <si>
     <t>JUMPER</t>
   </si>
   <si>
-    <t>20.155MH/2</t>
-  </si>
-  <si>
     <t>1658621-1</t>
   </si>
   <si>
@@ -181,6 +160,30 @@
   </si>
   <si>
     <t>C1, C2</t>
+  </si>
+  <si>
+    <t>B3F-4000</t>
+  </si>
+  <si>
+    <t>TERMINAL BLOCK PLUG 8WAY</t>
+  </si>
+  <si>
+    <t>TERMINAL BLOCK PLUG 2WAY</t>
+  </si>
+  <si>
+    <t>3365/10 100</t>
+  </si>
+  <si>
+    <t>691361100002</t>
+  </si>
+  <si>
+    <t>691322110002</t>
+  </si>
+  <si>
+    <t>691322110008</t>
+  </si>
+  <si>
+    <t>691361100008</t>
   </si>
 </sst>
 </file>
@@ -724,7 +727,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -741,10 +744,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1111,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,21 +1150,21 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1169,19 +1173,19 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1190,28 +1194,28 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -1226,10 +1230,10 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1301.9306999999999</v>
+        <v>31</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
@@ -1257,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1274,13 +1278,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
@@ -1291,37 +1295,37 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="A11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
+        <v>44</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1329,10 +1333,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1340,47 +1344,49 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">

</xml_diff>